<commit_message>
multiple page data write in one excel file
</commit_message>
<xml_diff>
--- a/mobile_data.xlsx
+++ b/mobile_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1315,6 +1315,846 @@
         </is>
       </c>
     </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Vivo</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>৳25,000.00</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>2024, April 29</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Android 14, OriginOS 4</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>6.78" 1260x2800 pixels</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>50MP 2160p</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>8/12GB RAM Snapdragon 7 Gen 3</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>6000mAh 80W</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Vivo</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>৳35,000.00</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>2024, April 29</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Android 14, OriginOS 4</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>6.78" 1260x2800 pixels</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>50MP 2160p</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>12/16GB RAM Snapdragon 8s Gen 3</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>6000mAh 80W</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Vivo</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>৳20,000.00</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>2024, April 29</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Android 14, OriginOS 4</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>6.72" 1080x2408 pixels</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>50MP 2160p</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>8/12GB RAM Snapdragon 6 Gen 1</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>6000mAh 44W</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Realme</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>৳18,000.00</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>2024, April 24</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Android 14, Realme UI 5.0</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>6.72" 1080x2400 pixels</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>50MP 1080p</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>6.72" 1080x2400 pixels</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>5000mAh 45W</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Infinix</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Coming soon</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Not announced yet</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Android 13</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>6.78" 1080x2400 pixels</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>108MP 1440p</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>4/8GB RAM Dimensity 7020</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>5000mAh Li-Po</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Realme</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>৳20,000.00</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>2024, April 25</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Android 14, Realme UI 5.0</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>6.67" 1080x2400 pixels</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>50MP 1080p</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>6/8GB RAM Dimensity 7050</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>5000mAh 45W</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Oppo</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>৳32,000.00</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>2024, April 29</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Android 14, ColorOS 14</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>6.7" 1080x2412 pixels</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>50MP 2160p</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>8/12GB RAM Snapdragon 7 Gen 3</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>5500mAh 100W</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>HMD</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>৳25,000.00</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>2024, April</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Android 14</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>6.56" 720x1480 pixels</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>50MP 1080p</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>4-8GB RAM Unisoc T606</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>5000mAh 20W</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Nothing</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Coming soon</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Not announced yet</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Android 14</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>6.55" 1440x3216 pixels</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>50MP 2160p</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>8/12GB RAM Snapdragon 778G+ 5G</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>4500mAh Li-Po</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Vivo</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Coming soon</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Not announced yet</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Android 14</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>6.78" 1440x3200 pixels</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>64MP 4320p</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>16GB RAM Snapdragon 8 Gen 3</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>5100mAh Li-Po</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Vivo</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Coming soon</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Not announced yet</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Android 14</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>6.78" 1260x2800 pixels</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>64MP 4320p</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>12/16GB RAM Snapdragon 8 Gen 3</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>5000mAh Li-Po</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Motorola</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Coming soon</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Not announced yet</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Android 13</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>6.5" 720x1600 pixels</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>13MP 1080p</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>2/4GB RAM Unisoc T606</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>5000mAh Li-Po</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Huawei</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>৳160,000.00</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>2024, April 29</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>HarmonyOS 4.2</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>6.8" 1260x2844 pixels</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>50MP 2160p</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>16GB RAM Kirin 9010</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>5200mAh 100W80W</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Huawei</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>৳120,000.00</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Exp. release 2024, April 29</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>HarmonyOS 4.2</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>6.8" 1260x2844 pixels</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>50MP 2160p</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>16GB RAM Kirin 9010</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>5050mAh 100W 80W</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Huawei</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>৳100,000.00</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>2024, April 29</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>HarmonyOS 4.2</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>6.8" 1260x2844 pixels</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>50MP 2160p</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>12GB RAM Kirin 9010</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>5050mAh 100W 80W</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Huawei</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>৳85,000.00</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Exp. release 2024, May 06</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>EMUI 14.2, HarmonyOS 4.2</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>6.6" 1256x2760 pixels</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>50MP 2160p</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>12GB RAM Kirin 9010</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>4900mAh 66W 50W</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>HMD</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>৳18,000.00</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>2024, April 24</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Android 14</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>6.65" 720x1612 pixels</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>13MP 1080p</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>4/6GB RAM Unisoc T606</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>5000mAh Li-Po</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Vivo</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>৳18,000.00</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>2024, April 24</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Android 14, Funtouch 14</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>6.72" 1080x2408 pixels</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>50MP 2160p</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>4-8GB RAM Snapdragon 6 Gen 1</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>6000mAh 44W</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Vivo</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>৳25,000.00</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>2024, April 27</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Android 14, OriginOS 4</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>6.72" 1080x2408 pixels</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>50MP 1080p</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>8/12GB RAM Snapdragon 4 Gen 2</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>6000mAh 44W</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Motorola</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>৳120,000.00</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Exp. release 2024, April</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Android 14</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>6.7" 1220x2712 pixels</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>50MP 4320p</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>12/16GB RAM Snapdragon 8s Gen 3</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>5000mAh 125W 50W</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
scrape discount items properly
</commit_message>
<xml_diff>
--- a/mobile_data.xlsx
+++ b/mobile_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H41"/>
+  <dimension ref="A1:H101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2155,6 +2155,2526 @@
         </is>
       </c>
     </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Motorola</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Coming soon</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Not announced yet</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Android 13</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>6.5" 1080x2400 pixels</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>50MP 1080p</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>12GB RAM Snapdragon 695 5G</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>5000mAh Li-Po</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Vivo</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>৳15,000.00</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>2024, May 03</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Android 14, Funtouch 14</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>6.56" 720x1612 pixels</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>50MP 1080p</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>4GB RAM Helio G85</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>5000mAh 15W</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Vivo</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>৳30,000.00</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>2024, May 03</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Android 14, Funtouch 14</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>6.67" 1080x2400 pixels</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>50MP 1080p</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>8GB RAM Snapdragon 685</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>5000mAh 80W</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Vivo</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Coming soon</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Exp. release 2024, May</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Android 14, Funtouch 14</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>6.68" 720x1612 pixels</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>50MP 1080p</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>8GB RAM Snapdragon 4 Gen 2</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>6000mAh 44W</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Vivo</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>৳40,000.00</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Exp. release 2024, May 09</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>Android 14, Funtouch 14</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>6.78" 1080x2400 pixels</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>50MP 2160p</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>8GB RAM Snapdragon 6 Gen 1</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>5500mAh 44W</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Vivo</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>৳30,000.00</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>2024, May 01</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Android 14, Funtouch 14</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>6.67" 1080x2400 pixels</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>50MP 1080p</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>8GB RAM Snapdragon 4 Gen 2</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>5000mAh 44W</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Xiaomi</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Coming soon</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Not announced yet</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Android 14</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>6.28" 1080x2400 pixels</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>50MP 4320p</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>8/12GB RAM Snapdragon 8 Gen1</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>4500mAh Li-Po</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>HTC</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Coming soon</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Not announced yet</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>Android 13</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>6.7" 1080x2400 pixels</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>108MP 2160p</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>8/12GB RAM Snapdragon 7 Gen 1</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>4600mAh Li-Po</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>HMD</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Coming soon</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Not announced yet</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Android 14</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>6.49" 1080x2400 pixels</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>64MP 2160p</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>6GB RAM Snapdragon 695 5G</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>4800mAh Li-Po</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Vivo</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Coming soon</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Not announced yet</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Android 13</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>6.51" 720x1600 pixels</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>13MP 1080p</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>4-8GB RAM Dimensity 700</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>5000mAh Li-Po</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Energizer</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>৳10,000.00</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Exp. release 2024, July</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Android 13</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>6.51" 720x1600 pixels</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>18MP 1080p</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>2GB RAM MT6739WW</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>4000mAh</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Vivo</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Coming soon</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Exp. release 2024, May</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>Android 14, Funtouch 14</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>6.56" 720x1612 pixels</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>13MP 1080p</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>4GB RAM Helio G85</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>5000mAh 15W</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Realme</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>৳15,000.00</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>2024, April 26</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>Android 14, Realme UI 5.0</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>6.67" 720x1604 pixels</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>50MP 1080p</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>4/6GB RAM Dimensity 6300</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>5000mAh 15W</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Infinix</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>৳32,000.00</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>2024, April 26</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>Android 14, XOS 14</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>6.78" 1080x2400 pixels</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>108MP 2160p</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>8/12GB RAM Dimensity 8200</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>5000mAh 45W</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Oppo</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Coming soon</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>2024, April 26</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>Android 14, ColorOS 14</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>6.67" 720x1604 pixels</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>50MP 1080p</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>8GB RAM Snapdragon 680 4G</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>5000mAh 45W</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Xiaomi</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Coming soon</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Not announced yet</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>Android 13</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>6.74" 720x1650 pixels</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>50MP 1080p</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>4-8GB RAM Dimensity 6100+</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>5000mAh Li-Po</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Xiaomi</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Coming soon</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Not announced yet</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>Android 14</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>6.53" 1080x2340 pixels</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>64MP 1080p</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>6GB RAM Snapdragon 662</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>4500mAh Li-Po</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Polestar</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Coming soon</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>2024, April 24</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>Polestar OS</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>6.79" 1368x3192 pixels</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>50MP 1080p</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>16GB RAM Snapdragon 8 Gen 3</t>
+        </is>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>5050mAh 80W 50W</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>HMD</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Coming soon</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Exp. release 2024, April</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>Android 14</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>6.56" 720x1480 pixels</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>13MP 1080p</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>4GB RAM Snapdragon 680 4G</t>
+        </is>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>4000mAh 10W</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>HMD</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>৳20,000.00</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Exp. release 2024, April</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>Android 14</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>6.65" 720x1612 pixels</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>50MP 1080p</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>4-8GB RAM Unisoc T606</t>
+        </is>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>5000mAh 10W</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>Samsung</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Coming soon</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Not announced yet</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>Android 14</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>6.4" 1080x2340 pixels</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>50MP 4320p</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>8GB RAM Exynos 2200</t>
+        </is>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>4500mAh Li-Ion</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>Honor</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Coming soon</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Exp. release 2024, April</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>Android 13, MagicOS 7.2</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>6.8" 1080x2412 pixels</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>100MP 1080p</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>8GB RAM Dimensity 6020</t>
+        </is>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>6000mAh 35W</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>Vivo</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>৳35,000.00</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>2024, April 04</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>Android 14, Funtouch 14</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>6.67" 1080x2400 pixels</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>50MP 1080p</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>8GB RAM Snapdragon 685</t>
+        </is>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>5000mAh 80W</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>Tecno</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Coming soon</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Exp. release 2024, April</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>Android 14, HIOS 14</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>6.78" 1080x2460 pixels</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>50MP 1440p</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>8GB RAM Helio G99 Ultimate</t>
+        </is>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>7000mAh 33W</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>Tecno</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Coming soon</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Exp. release 2024, April</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>Android 14, HIOS 14</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>6.78" 1080x2460 pixels</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>108MP 1080p</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>8/12GB RAM Helio G99 Ultimate</t>
+        </is>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>6000mAh 70W</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>Vivo</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Coming soon</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Not announced yet</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>Android 14</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>6.78" 1260x2800 pixels</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>50MP 4320p</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>12/16GB RAM Snapdragon 8 Gen 2</t>
+        </is>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>5160mAh</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>Motorola</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>৳46,000.00</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>2024, April 8</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>Android 14</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>6.7" 1080x2400 pixels</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>50MP 4320p</t>
+        </is>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>8/12GB RAM Snapdragon 7 Gen 3</t>
+        </is>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>4500mAh 125W 50W</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>Realme</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>৳20,000.00</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>2024, April 02</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>Android 14, Realme UI 5.0</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>6.72" 1080x2400 pixels</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>50MP 1080p</t>
+        </is>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>4/8GB RAM Dimensity 6100+</t>
+        </is>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>5000mAh 45W</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>Realme</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>৳18,000.00</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>2024, April</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>Android 14, Realme UI 5.0</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>6.67" 720x1604 pixels</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>50MP 1080p</t>
+        </is>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>6/8GB RAM Helio G85</t>
+        </is>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>5000mAh 45W</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>Xiaomi</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>Coming soon</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Not announced yet</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>Android 14</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>6.67" 1220x2712 pixels</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>64MP 2160p</t>
+        </is>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>8/12GB RAM Dimensity 8300 Ultra</t>
+        </is>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>5000mAh</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>Xiaomi</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>Coming soon</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>Not announced yet</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>Android 14</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>6.67" 1220x2712 pixels</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>64MP 2160p</t>
+        </is>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>8/12GB RAM Snapdragon 7s Gen 2</t>
+        </is>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>5100mAh</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>Infinix</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>Coming soon</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>Not announced yet</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>Android 14</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>6.78" 1080x2436 pixels</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>108MP 1440p</t>
+        </is>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>8GB RAM Dimensity 7020</t>
+        </is>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>5000mAh 45W20W</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>Infinix</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>Coming soon</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Not announced yet</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>Android 14</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>6.78" 1080x2436 pixels</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>108MP 1440p</t>
+        </is>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>8GB RAM Helio G99 Ultimate</t>
+        </is>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>5000mAh 45W20W</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>Realme</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>Coming soon</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>Not announced yet</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>Android 14</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>6.74" 1080x2400 pixels</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>50MP 1080p</t>
+        </is>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>4/6GB RAM Unisoc Tiger T612</t>
+        </is>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>5000mAh Li-Po</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>OnePlus</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>৳37,500.00</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>2024, April 04</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>Android 14, ColorOS 14</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>6.7" 1080x2412 pixels</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>50MP 2160p</t>
+        </is>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>8GB RAM Snapdragon 7 Gen 3</t>
+        </is>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>5500mAh 100W</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>Xiaomi</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>Coming soon</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>Not announced yet</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>Android 14</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>6.52" 720x1600 pixels</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>8MP 1080p</t>
+        </is>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>2-4GB RAM Helio G36</t>
+        </is>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>5000mAh Li-Po</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>Vivo</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>Coming soon</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>Not announced yet</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>Android 13</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>6.4" 1080x2400 pixels</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>64MP 2160p</t>
+        </is>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>6GB RAM Snapdragon 720G</t>
+        </is>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>5000mAh Li-Po</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>Realme</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>Coming soon</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>Not announced yet</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>Android 14</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>6.78" 1264x2780 pixels</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>50MP 2160p</t>
+        </is>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>12/16GB RAM Snapdragon 8 Gen 3</t>
+        </is>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>5400mAh Li-Po</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>Realme</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>Coming soon</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>Not announced yet</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>Android 14</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>6.74" 1240x2772 pixels</t>
+        </is>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>50MP 2160p</t>
+        </is>
+      </c>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>12/16GB RAM Snapdragon 8 Gen 2</t>
+        </is>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>5240mAh Li-Po</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>Honor</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>Coming soon</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>Not announced yet</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>Android 13</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>6.56" 720x1612 pixels</t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>13MP 1080p</t>
+        </is>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>6/8GB RAM Snapdragon 480+ 5G</t>
+        </is>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>4500mAh Li-Po</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>Motorola</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>৳120,000.00</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>Exp. release 2024, April</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>Android 14</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>6.7" 1220x2712 pixels</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>50MP 4320p</t>
+        </is>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>12/16GB RAM Snapdragon 8s Gen 3</t>
+        </is>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>5000mAh 125W 50W</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>Motorola</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>৳45,000.00</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>Exp. release 2024, April</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>Android 14</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>6.7" 1080x2400 pixels</t>
+        </is>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>50MP 2160p</t>
+        </is>
+      </c>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>8/12GB RAM Snapdragon 7s Gen 2</t>
+        </is>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>5000mAh 68W</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>Huawei</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>Coming soon</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>Not announced yet</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>HarmonyOS 3.1</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>6.67" 1220x2700 pixels</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>48MP 2160p</t>
+        </is>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>12GB RAM Snapdragon 8+ Gen 1 4G</t>
+        </is>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>5100mAh</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>Realme</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>৳30,000.00</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>2024, April 22</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>Android 14, Realme UI 5.0</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>6.7" 1080x2412 pixels</t>
+        </is>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>50MP 2160p</t>
+        </is>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>8GB RAM Snapdragon 6 Gen 1</t>
+        </is>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>5000mAh 45W</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>Realme</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>৳26,000.00</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>2024, April 15</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>Android 14, Realme UI 5.0</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>6.67" 1080x2400 pixels</t>
+        </is>
+      </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>50MP 1080p</t>
+        </is>
+      </c>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>6/8GB RAM Dimensity 7050</t>
+        </is>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>5000mAh 45W</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>Tecno</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>Coming soon</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>Not announced yet</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>Android 13</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>6.9" 1080x2640 pixels</t>
+        </is>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>64MP 2160p</t>
+        </is>
+      </c>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t>8GB RAM Dimensity 8050</t>
+        </is>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>4000mAh Li-Po</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>Vivo</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>Coming soon</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>Not announced yet</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>Android 13</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>6.78" 1440x3200 pixels</t>
+        </is>
+      </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>64MP 4320p</t>
+        </is>
+      </c>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>12GB RAM Snapdragon 8 Gen 2</t>
+        </is>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>5000mAh Li-Po</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>Oppo</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>৳35,000.00</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>2024, April 19</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>Android 14, ColorOS 14</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>6.7" 1080x2412 pixels</t>
+        </is>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>64MP 2160p</t>
+        </is>
+      </c>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>8/12GB RAM Dimensity 7050</t>
+        </is>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>5000mAh 67W</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>ZTE</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>Coming soon</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>Exp. release 2024, Q2-Q4</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>Android 14</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>6.78" 1260x2800 pixels</t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>50MP 4320p</t>
+        </is>
+      </c>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>12GB RAM Snapdragon 8 Gen 2</t>
+        </is>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>6000mAh 80W</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>Realme</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>৳50,000.00</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>2024, April 17</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>Android 14, Realme UI 5.0</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>6.78" 1264x2780 pixels</t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>50MP 2160p</t>
+        </is>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>8-16GB RAM Snapdragon 7+ Gen 3</t>
+        </is>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>5500mAh 100W</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>Cubot</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>৳25,000.00</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>2024, April</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>Android 14</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>6.58" 1080x2408 pixels</t>
+        </is>
+      </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>64MP 1080p</t>
+        </is>
+      </c>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t>8GB RAM MT8788V</t>
+        </is>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>4350mAh 18W</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>Cubot</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>৳40,000.00</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>2024, April</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>Android 13</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>6.67" 1080x2400 pixels</t>
+        </is>
+      </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>100MP 1080p</t>
+        </is>
+      </c>
+      <c r="G93" t="inlineStr">
+        <is>
+          <t>12GB RAM Helio G99</t>
+        </is>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>5100mAh 33W</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>Cubot</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>৳30,000.00</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>2024, April</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>Android 14</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>6.58" 1080x2408 pixels</t>
+        </is>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>100MP 1080p</t>
+        </is>
+      </c>
+      <c r="G94" t="inlineStr">
+        <is>
+          <t>12GB RAM Helio G99</t>
+        </is>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>5100mAh 33W</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>Cubot</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>৳15,000.00</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>2024, April</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>Android 13</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>6.56" 720x1612 pixels</t>
+        </is>
+      </c>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>13MP 1080p</t>
+        </is>
+      </c>
+      <c r="G95" t="inlineStr">
+        <is>
+          <t>4GB RAM Unisoc SC9863A</t>
+        </is>
+      </c>
+      <c r="H95" t="inlineStr">
+        <is>
+          <t>5100mAh 10W</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>Motorola</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>৳20,000.00</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>2024, April 09</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>Android 14</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>6.56" 720x1612 pixels</t>
+        </is>
+      </c>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>50MP 1080p</t>
+        </is>
+      </c>
+      <c r="G96" t="inlineStr">
+        <is>
+          <t>4/8GB RAM Unisoc T606</t>
+        </is>
+      </c>
+      <c r="H96" t="inlineStr">
+        <is>
+          <t>5000mAh 15W</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>Xiaomi</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>৳42,000.00</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>2024, April 10</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>Android 14, HyperOS</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>6.67" 1220x2712 pixels</t>
+        </is>
+      </c>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>50MP 4320p</t>
+        </is>
+      </c>
+      <c r="G97" t="inlineStr">
+        <is>
+          <t>12/16GB RAM Snapdragon 8s Gen 3</t>
+        </is>
+      </c>
+      <c r="H97" t="inlineStr">
+        <is>
+          <t>5000mAh 90W</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>Motorola</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>৳25,000.00</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>2024, April 23</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>Android 14, planned upgrade to Android 15</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>6.5" 1080x2400 pixels</t>
+        </is>
+      </c>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>50MP 1080p</t>
+        </is>
+      </c>
+      <c r="G98" t="inlineStr">
+        <is>
+          <t>8/12GB RAM Dimensity 7025</t>
+        </is>
+      </c>
+      <c r="H98" t="inlineStr">
+        <is>
+          <t>6000mAh 30W</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>Honor</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>৳30,000.00</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>2024, April 12</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>Android 13, Magic OS 7.2</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>6.8" 1080x2412 pixels</t>
+        </is>
+      </c>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>108MP 1080p</t>
+        </is>
+      </c>
+      <c r="G99" t="inlineStr">
+        <is>
+          <t>4GB RAM Dimensity 6020</t>
+        </is>
+      </c>
+      <c r="H99" t="inlineStr">
+        <is>
+          <t>5330mAh 35W</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>Realme</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>Coming soon</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>Not announced yet</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>Android 14, Realme UI 5.0</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>6.67" 720x1604 pixels</t>
+        </is>
+      </c>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t>5MP 1080p</t>
+        </is>
+      </c>
+      <c r="G100" t="inlineStr">
+        <is>
+          <t>6/8GB RAM Helio G85</t>
+        </is>
+      </c>
+      <c r="H100" t="inlineStr">
+        <is>
+          <t>5000mAh 45W</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>Oukitel</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>৳22,000.00</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>Exp. release 2024, April</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>Android 13</t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>6.6" 1080x2408 pixels</t>
+        </is>
+      </c>
+      <c r="F101" t="inlineStr">
+        <is>
+          <t>64MP 1440p</t>
+        </is>
+      </c>
+      <c r="G101" t="inlineStr">
+        <is>
+          <t>8GB RAM Dimensity 6100+</t>
+        </is>
+      </c>
+      <c r="H101" t="inlineStr">
+        <is>
+          <t>11000mAh Li-Po</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>